<commit_message>
refactor: improoved excel file generation (column default sort)
</commit_message>
<xml_diff>
--- a/resources/calculate.xlsx
+++ b/resources/calculate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Privat\git\se-mods\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Privat\git\se-mods\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61990A2-2D0A-47DB-B54E-D1BE0D01290C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{935D1D37-8EEF-4D51-AF47-EDD77E32BC25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ewe-core-minerals-oreToIngot" sheetId="1" r:id="rId1"/>
@@ -599,7 +599,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -773,6 +773,12 @@
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -790,12 +796,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1138,7 +1138,7 @@
   <dimension ref="A1:DC118"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q105" sqref="Q105:Q118"/>
+      <selection activeCell="F104" sqref="F104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4422,26 +4422,26 @@
       </c>
     </row>
     <row r="85" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="G85" s="33" t="s">
+      <c r="G85" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="H85" s="33"/>
-      <c r="I85" s="32" t="s">
+      <c r="H85" s="37"/>
+      <c r="I85" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="J85" s="32"/>
-      <c r="K85" s="31" t="s">
+      <c r="J85" s="36"/>
+      <c r="K85" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="L85" s="31"/>
-      <c r="M85" s="30" t="s">
+      <c r="L85" s="35"/>
+      <c r="M85" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="N85" s="30"/>
-      <c r="O85" s="28" t="s">
+      <c r="N85" s="34"/>
+      <c r="O85" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="P85" s="29"/>
+      <c r="P85" s="33"/>
       <c r="Q85" s="3"/>
       <c r="R85" s="3"/>
     </row>
@@ -5027,7 +5027,7 @@
       <c r="N104" t="s">
         <v>167</v>
       </c>
-      <c r="O104" s="37">
+      <c r="O104" s="31">
         <v>18800</v>
       </c>
       <c r="P104">
@@ -5057,10 +5057,10 @@
       <c r="O105" t="s">
         <v>169</v>
       </c>
-      <c r="P105" s="34">
+      <c r="P105" s="28">
         <v>0.78600000000000003</v>
       </c>
-      <c r="Q105" s="36">
+      <c r="Q105" s="30">
         <f>O104*(1-SUM(P107:P118))*P105</f>
         <v>11998.7616</v>
       </c>
@@ -5092,10 +5092,10 @@
       <c r="O106" t="s">
         <v>169</v>
       </c>
-      <c r="P106" s="34">
+      <c r="P106" s="28">
         <v>0.214</v>
       </c>
-      <c r="Q106" s="36">
+      <c r="Q106" s="30">
         <f>O104*(1-SUM(P107:P118))*P106</f>
         <v>3266.8383999999996</v>
       </c>
@@ -5127,10 +5127,10 @@
       <c r="O107" t="s">
         <v>169</v>
       </c>
-      <c r="P107" s="34">
+      <c r="P107" s="28">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="Q107" s="35">
+      <c r="Q107" s="29">
         <f>O$104*P107</f>
         <v>1410</v>
       </c>
@@ -5162,10 +5162,10 @@
       <c r="O108" t="s">
         <v>169</v>
       </c>
-      <c r="P108" s="34">
+      <c r="P108" s="28">
         <v>0.04</v>
       </c>
-      <c r="Q108" s="35">
+      <c r="Q108" s="29">
         <f t="shared" ref="Q108:Q118" si="16">O$104*P108</f>
         <v>752</v>
       </c>
@@ -5203,10 +5203,10 @@
       <c r="O109" t="s">
         <v>169</v>
       </c>
-      <c r="P109" s="34">
+      <c r="P109" s="28">
         <v>0.02</v>
       </c>
-      <c r="Q109" s="35">
+      <c r="Q109" s="29">
         <f t="shared" si="16"/>
         <v>376</v>
       </c>
@@ -5244,10 +5244,10 @@
       <c r="O110" t="s">
         <v>169</v>
       </c>
-      <c r="P110" s="34">
+      <c r="P110" s="28">
         <v>0.01</v>
       </c>
-      <c r="Q110" s="35">
+      <c r="Q110" s="29">
         <f t="shared" si="16"/>
         <v>188</v>
       </c>
@@ -5285,10 +5285,10 @@
       <c r="O111" t="s">
         <v>169</v>
       </c>
-      <c r="P111" s="34">
+      <c r="P111" s="28">
         <v>0.01</v>
       </c>
-      <c r="Q111" s="35">
+      <c r="Q111" s="29">
         <f t="shared" si="16"/>
         <v>188</v>
       </c>
@@ -5326,10 +5326,10 @@
       <c r="O112" t="s">
         <v>169</v>
       </c>
-      <c r="P112" s="34">
+      <c r="P112" s="28">
         <v>0.01</v>
       </c>
-      <c r="Q112" s="35">
+      <c r="Q112" s="29">
         <f t="shared" si="16"/>
         <v>188</v>
       </c>
@@ -5352,10 +5352,10 @@
       <c r="O113" t="s">
         <v>169</v>
       </c>
-      <c r="P113" s="34">
+      <c r="P113" s="28">
         <v>0.01</v>
       </c>
-      <c r="Q113" s="35">
+      <c r="Q113" s="29">
         <f t="shared" si="16"/>
         <v>188</v>
       </c>
@@ -5378,10 +5378,10 @@
       <c r="O114" t="s">
         <v>169</v>
       </c>
-      <c r="P114" s="34">
+      <c r="P114" s="28">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="Q114" s="35">
+      <c r="Q114" s="29">
         <f t="shared" si="16"/>
         <v>94</v>
       </c>
@@ -5404,10 +5404,10 @@
       <c r="O115" t="s">
         <v>169</v>
       </c>
-      <c r="P115" s="34">
+      <c r="P115" s="28">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="Q115" s="35">
+      <c r="Q115" s="29">
         <f t="shared" si="16"/>
         <v>94</v>
       </c>
@@ -5430,10 +5430,10 @@
       <c r="O116" t="s">
         <v>169</v>
       </c>
-      <c r="P116" s="34">
+      <c r="P116" s="28">
         <v>1E-3</v>
       </c>
-      <c r="Q116" s="35">
+      <c r="Q116" s="29">
         <f t="shared" si="16"/>
         <v>18.8</v>
       </c>
@@ -5456,10 +5456,10 @@
       <c r="O117" t="s">
         <v>169</v>
       </c>
-      <c r="P117" s="34">
+      <c r="P117" s="28">
         <v>1E-3</v>
       </c>
-      <c r="Q117" s="35">
+      <c r="Q117" s="29">
         <f t="shared" si="16"/>
         <v>18.8</v>
       </c>
@@ -5482,10 +5482,10 @@
       <c r="O118" t="s">
         <v>169</v>
       </c>
-      <c r="P118" s="34">
+      <c r="P118" s="28">
         <v>1E-3</v>
       </c>
-      <c r="Q118" s="35">
+      <c r="Q118" s="29">
         <f t="shared" si="16"/>
         <v>18.8</v>
       </c>

</xml_diff>